<commit_message>
Update PM08 Tidsregistrering for Benjamin.xlsx
</commit_message>
<xml_diff>
--- a/08 Project Management/Tidsregistrering/PM08 Tidsregistrering for Benjamin.xlsx
+++ b/08 Project Management/Tidsregistrering/PM08 Tidsregistrering for Benjamin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benky\OneDrive\IdeaProjects\HoeKulator\08 Project Management\Tidsregistrering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benky\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="8_{468DB78F-210C-4DB9-B277-7CC0D8D841D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{266BC9FC-221E-40F3-86FB-843E14B200B2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B78E9B-9D0A-484D-843F-3E2C2EF28DE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8964" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="Roller">'Ark2'!$B$3:$B$31</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
   <si>
     <t>Tidsregistrering af (Navn)</t>
   </si>
@@ -165,10 +168,28 @@
     <t>1 time</t>
   </si>
   <si>
-    <t>Oprette risikoanalyse</t>
-  </si>
-  <si>
     <t>3 timer</t>
+  </si>
+  <si>
+    <t>10 min</t>
+  </si>
+  <si>
+    <t>Review af SSD01 Beregn Omsætning'</t>
+  </si>
+  <si>
+    <t>Lav AD08 Beregn Afskrivning</t>
+  </si>
+  <si>
+    <t>Indsaml test data til UC08 Beregn Afskrivning</t>
+  </si>
+  <si>
+    <t>Lav risikoanalyse</t>
+  </si>
+  <si>
+    <t>1t 30min</t>
+  </si>
+  <si>
+    <t>Lav vejledninger til branching i GitHub og  GitHub Desktop</t>
   </si>
 </sst>
 </file>
@@ -319,7 +340,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -344,10 +365,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -364,13 +381,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -399,7 +428,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>60960</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>68580</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184731" cy="264560"/>
@@ -750,34 +779,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07EC185-8A27-41F3-967D-179793E73F80}">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="53.88671875" style="11" customWidth="1"/>
-    <col min="3" max="3" width="31.44140625" style="18" customWidth="1"/>
-    <col min="4" max="4" width="26.77734375" style="17" customWidth="1"/>
-    <col min="5" max="5" width="31" style="17" customWidth="1"/>
-    <col min="6" max="6" width="31" style="21" customWidth="1"/>
+    <col min="3" max="3" width="31.44140625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="26.77734375" style="15" customWidth="1"/>
+    <col min="5" max="5" width="31" style="15" customWidth="1"/>
+    <col min="6" max="6" width="31" style="19" customWidth="1"/>
     <col min="7" max="7" width="37.21875" style="6" customWidth="1"/>
     <col min="8" max="8" width="37.21875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
@@ -795,7 +824,7 @@
       <c r="E2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="17" t="s">
         <v>35</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -806,451 +835,523 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A3" s="11" t="s">
-        <v>41</v>
+      <c r="A3" s="21" t="s">
+        <v>46</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="12">
-        <v>43885</v>
-      </c>
-      <c r="D3" s="13">
-        <v>0.38541666666666669</v>
-      </c>
-      <c r="E3" s="14">
-        <v>0.4201388888888889</v>
-      </c>
-      <c r="F3" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="5">
-        <f>E3-D3</f>
-        <v>3.472222222222221E-2</v>
-      </c>
-      <c r="H3" s="1">
-        <f>SUM(G$3:G3)</f>
-        <v>3.472222222222221E-2</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C3" s="13">
+        <v>43881</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A4" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="13">
+        <v>43881</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="13">
+        <v>43885</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="5">
+        <f>E5-D5</f>
+        <v>3.472222222222221E-2</v>
+      </c>
+      <c r="H5" s="1">
+        <f>SUM(G$5:G5)</f>
+        <v>3.472222222222221E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="13">
+        <v>43885</v>
+      </c>
+      <c r="D6" s="14">
+        <v>0.4375</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="G6" s="5">
+        <f>E6-D6</f>
+        <v>0.22916666666666663</v>
+      </c>
+      <c r="H6" s="1">
+        <f>SUM(G$5:G6)</f>
+        <v>0.26388888888888884</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="15">
-        <v>43885</v>
-      </c>
-      <c r="D4" s="16">
-        <v>0.4375</v>
-      </c>
-      <c r="E4" s="16">
+      <c r="C7" s="13">
+        <v>43886</v>
+      </c>
+      <c r="D7" s="14">
+        <v>0.375</v>
+      </c>
+      <c r="E7" s="14">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="5">
+        <f>E7-D7</f>
+        <v>5.555555555555558E-2</v>
+      </c>
+      <c r="H7" s="1">
+        <f>SUM(G$5:G7)</f>
+        <v>0.31944444444444442</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A8" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="13">
+        <v>43886</v>
+      </c>
+      <c r="D8" s="14">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="E8" s="14">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="5">
+        <f>E8-D8</f>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="H8" s="1">
+        <f>SUM(G$5:G8)</f>
+        <v>0.3298611111111111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A9" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="13">
+        <v>43886</v>
+      </c>
+      <c r="D9" s="14">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="E9" s="14">
         <v>0.66666666666666663</v>
       </c>
-      <c r="F4" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" s="5">
-        <f t="shared" ref="G4:G32" si="0">E4-D4</f>
-        <v>0.22916666666666663</v>
-      </c>
-      <c r="H4" s="1">
-        <f>SUM(G$3:G4)</f>
-        <v>0.26388888888888884</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
-        <f>SUM(G$3:G5)</f>
-        <v>0.26388888888888884</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
-        <f>SUM(G$3:G6)</f>
-        <v>0.26388888888888884</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="1">
-        <f>SUM(G$3:G7)</f>
-        <v>0.26388888888888884</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H8" s="1">
-        <f>SUM(G$3:G8)</f>
-        <v>0.26388888888888884</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="20"/>
+      <c r="F9" s="18" t="s">
+        <v>49</v>
+      </c>
       <c r="G9" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="G9:G34" si="0">E9-D9</f>
+        <v>0.15277777777777768</v>
       </c>
       <c r="H9" s="1">
-        <f>SUM(G$3:G9)</f>
-        <v>0.26388888888888884</v>
+        <f>SUM(G$5:G9)</f>
+        <v>0.48263888888888878</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="20"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="18"/>
       <c r="G10" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H10" s="1">
-        <f>SUM(G$3:G10)</f>
-        <v>0.26388888888888884</v>
+        <f>SUM(G$5:G10)</f>
+        <v>0.48263888888888878</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="20"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="18"/>
       <c r="G11" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H11" s="1">
-        <f>SUM(G$3:G11)</f>
-        <v>0.26388888888888884</v>
+        <f>SUM(G$5:G11)</f>
+        <v>0.48263888888888878</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C12" s="15"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="20"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="18"/>
       <c r="G12" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H12" s="1">
-        <f>SUM(G$3:G12)</f>
-        <v>0.26388888888888884</v>
+        <f>SUM(G$5:G12)</f>
+        <v>0.48263888888888878</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="20"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="18"/>
       <c r="G13" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H13" s="1">
-        <f>SUM(G$3:G13)</f>
-        <v>0.26388888888888884</v>
+        <f>SUM(G$5:G13)</f>
+        <v>0.48263888888888878</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C14" s="15"/>
-      <c r="F14" s="20"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="18"/>
       <c r="G14" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H14" s="1">
-        <f>SUM(G$3:G14)</f>
-        <v>0.26388888888888884</v>
+        <f>SUM(G$5:G14)</f>
+        <v>0.48263888888888878</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C15" s="15"/>
-      <c r="F15" s="20"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="18"/>
       <c r="G15" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H15" s="1">
-        <f>SUM(G$3:G15)</f>
-        <v>0.26388888888888884</v>
+        <f>SUM(G$5:G15)</f>
+        <v>0.48263888888888878</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C16" s="15"/>
-      <c r="F16" s="20"/>
+      <c r="C16" s="13"/>
+      <c r="F16" s="18"/>
       <c r="G16" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H16" s="1">
-        <f>SUM(G$3:G16)</f>
-        <v>0.26388888888888884</v>
+        <f>SUM(G$5:G16)</f>
+        <v>0.48263888888888878</v>
       </c>
     </row>
     <row r="17" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C17" s="15"/>
-      <c r="F17" s="20"/>
+      <c r="C17" s="13"/>
+      <c r="F17" s="18"/>
       <c r="G17" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H17" s="1">
-        <f>SUM(G$3:G17)</f>
-        <v>0.26388888888888884</v>
+        <f>SUM(G$5:G17)</f>
+        <v>0.48263888888888878</v>
       </c>
     </row>
     <row r="18" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C18" s="15"/>
-      <c r="F18" s="20"/>
+      <c r="C18" s="13"/>
+      <c r="F18" s="18"/>
       <c r="G18" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H18" s="1">
-        <f>SUM(G$3:G18)</f>
-        <v>0.26388888888888884</v>
+        <f>SUM(G$5:G18)</f>
+        <v>0.48263888888888878</v>
       </c>
     </row>
     <row r="19" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C19" s="15"/>
-      <c r="F19" s="20"/>
+      <c r="C19" s="13"/>
+      <c r="F19" s="18"/>
       <c r="G19" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H19" s="1">
-        <f>SUM(G$3:G19)</f>
-        <v>0.26388888888888884</v>
+        <f>SUM(G$5:G19)</f>
+        <v>0.48263888888888878</v>
       </c>
     </row>
     <row r="20" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C20" s="15"/>
-      <c r="F20" s="20"/>
+      <c r="C20" s="13"/>
+      <c r="F20" s="18"/>
       <c r="G20" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H20" s="1">
-        <f>SUM(G$3:G20)</f>
-        <v>0.26388888888888884</v>
+        <f>SUM(G$5:G20)</f>
+        <v>0.48263888888888878</v>
       </c>
     </row>
     <row r="21" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C21" s="15"/>
-      <c r="F21" s="20"/>
+      <c r="C21" s="13"/>
+      <c r="F21" s="18"/>
       <c r="G21" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H21" s="1">
-        <f>SUM(G$3:G21)</f>
-        <v>0.26388888888888884</v>
+        <f>SUM(G$5:G21)</f>
+        <v>0.48263888888888878</v>
       </c>
     </row>
     <row r="22" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C22" s="15"/>
-      <c r="F22" s="20"/>
+      <c r="C22" s="13"/>
+      <c r="F22" s="18"/>
       <c r="G22" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H22" s="1">
-        <f>SUM(G$3:G22)</f>
-        <v>0.26388888888888884</v>
+        <f>SUM(G$5:G22)</f>
+        <v>0.48263888888888878</v>
       </c>
     </row>
     <row r="23" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C23" s="15"/>
-      <c r="F23" s="20"/>
+      <c r="C23" s="13"/>
+      <c r="F23" s="18"/>
       <c r="G23" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H23" s="1">
-        <f>SUM(G$3:G23)</f>
-        <v>0.26388888888888884</v>
+        <f>SUM(G$5:G23)</f>
+        <v>0.48263888888888878</v>
       </c>
     </row>
     <row r="24" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C24" s="15"/>
-      <c r="F24" s="20"/>
+      <c r="C24" s="13"/>
+      <c r="F24" s="18"/>
       <c r="G24" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H24" s="1">
-        <f>SUM(G$3:G24)</f>
-        <v>0.26388888888888884</v>
+        <f>SUM(G$5:G24)</f>
+        <v>0.48263888888888878</v>
       </c>
     </row>
     <row r="25" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C25" s="15"/>
+      <c r="C25" s="13"/>
+      <c r="F25" s="18"/>
       <c r="G25" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H25" s="1">
-        <f>SUM(G$3:G25)</f>
-        <v>0.26388888888888884</v>
+        <f>SUM(G$5:G25)</f>
+        <v>0.48263888888888878</v>
       </c>
     </row>
     <row r="26" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C26" s="15"/>
+      <c r="C26" s="13"/>
+      <c r="F26" s="18"/>
       <c r="G26" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H26" s="1">
-        <f>SUM(G$3:G26)</f>
-        <v>0.26388888888888884</v>
+        <f>SUM(G$5:G26)</f>
+        <v>0.48263888888888878</v>
       </c>
     </row>
     <row r="27" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C27" s="15"/>
+      <c r="C27" s="13"/>
       <c r="G27" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H27" s="1">
-        <f>SUM(G$3:G27)</f>
-        <v>0.26388888888888884</v>
+        <f>SUM(G$5:G27)</f>
+        <v>0.48263888888888878</v>
       </c>
     </row>
     <row r="28" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C28" s="15"/>
+      <c r="C28" s="13"/>
       <c r="G28" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H28" s="1">
-        <f>SUM(G$3:G28)</f>
-        <v>0.26388888888888884</v>
+        <f>SUM(G$5:G28)</f>
+        <v>0.48263888888888878</v>
       </c>
     </row>
     <row r="29" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C29" s="15"/>
+      <c r="C29" s="13"/>
       <c r="G29" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H29" s="1">
-        <f>SUM(G$3:G29)</f>
-        <v>0.26388888888888884</v>
+        <f>SUM(G$5:G29)</f>
+        <v>0.48263888888888878</v>
       </c>
     </row>
     <row r="30" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C30" s="15"/>
+      <c r="C30" s="13"/>
       <c r="G30" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H30" s="1">
-        <f>SUM(G$3:G30)</f>
-        <v>0.26388888888888884</v>
+        <f>SUM(G$5:G30)</f>
+        <v>0.48263888888888878</v>
       </c>
     </row>
     <row r="31" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C31" s="15"/>
+      <c r="C31" s="13"/>
       <c r="G31" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H31" s="1">
-        <f>SUM(G$3:G31)</f>
-        <v>0.26388888888888884</v>
+        <f>SUM(G$5:G31)</f>
+        <v>0.48263888888888878</v>
       </c>
     </row>
     <row r="32" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C32" s="15"/>
+      <c r="C32" s="13"/>
       <c r="G32" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H32" s="1">
-        <f>SUM(G$3:G32)</f>
-        <v>0.26388888888888884</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C33" s="15"/>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C34" s="15"/>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C35" s="15"/>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C36" s="15"/>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C37" s="15"/>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C38" s="15"/>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C39" s="15"/>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C40" s="15"/>
-    </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C41" s="15"/>
-    </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C42" s="15"/>
-    </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C43" s="15"/>
-    </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C44" s="15"/>
-    </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C45" s="15"/>
-    </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C46" s="15"/>
-    </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C47" s="15"/>
+        <f>SUM(G$5:G32)</f>
+        <v>0.48263888888888878</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C33" s="13"/>
+      <c r="G33" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H33" s="1">
+        <f>SUM(G$5:G33)</f>
+        <v>0.48263888888888878</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C34" s="13"/>
+      <c r="G34" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H34" s="1">
+        <f>SUM(G$5:G34)</f>
+        <v>0.48263888888888878</v>
+      </c>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C35" s="13"/>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C36" s="13"/>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C37" s="13"/>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C38" s="13"/>
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C39" s="13"/>
+    </row>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C40" s="13"/>
+    </row>
+    <row r="41" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C41" s="13"/>
+    </row>
+    <row r="42" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C42" s="13"/>
+    </row>
+    <row r="43" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C43" s="13"/>
+    </row>
+    <row r="44" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C44" s="13"/>
+    </row>
+    <row r="45" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C45" s="13"/>
+    </row>
+    <row r="46" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C46" s="13"/>
+    </row>
+    <row r="47" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C47" s="13"/>
+    </row>
+    <row r="48" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C48" s="13"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C49" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1289,13 +1390,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">

</xml_diff>